<commit_message>
H4MPT pathway in and precursors partway
</commit_message>
<xml_diff>
--- a/Matt_Work/Coenzyme Syntheses/synthesis pathway info.xlsx
+++ b/Matt_Work/Coenzyme Syntheses/synthesis pathway info.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832"/>
+    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coenzyme B" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="H4MPT" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="115">
   <si>
     <t>2-oxoglutarate + Acetyl-CoA -&gt;trans-homoaconitate</t>
   </si>
@@ -286,6 +286,81 @@
   </si>
   <si>
     <t>rxn10611</t>
+  </si>
+  <si>
+    <t>C9H11N5O6P</t>
+  </si>
+  <si>
+    <t>cpd15850</t>
+  </si>
+  <si>
+    <t>mptA</t>
+  </si>
+  <si>
+    <t>mptB</t>
+  </si>
+  <si>
+    <t>mptD</t>
+  </si>
+  <si>
+    <t>mptE</t>
+  </si>
+  <si>
+    <t>mptG</t>
+  </si>
+  <si>
+    <t>mptH</t>
+  </si>
+  <si>
+    <t>MMP0034</t>
+  </si>
+  <si>
+    <t>MMP0230</t>
+  </si>
+  <si>
+    <t>rxn10490</t>
+  </si>
+  <si>
+    <t>rxn03168</t>
+  </si>
+  <si>
+    <t>rxn02504</t>
+  </si>
+  <si>
+    <t>rxn02503</t>
+  </si>
+  <si>
+    <t>rxn10446</t>
+  </si>
+  <si>
+    <t>rn10491</t>
+  </si>
+  <si>
+    <t>MMP0243</t>
+  </si>
+  <si>
+    <t>MMP0579</t>
+  </si>
+  <si>
+    <t>MMP0279 (maybe)</t>
+  </si>
+  <si>
+    <t>GTP + 2 H2O -&gt; Formate + Ppi + 7,8-dihydronepterin 2' :3'-cyclicphosphate</t>
+  </si>
+  <si>
+    <t>7,8-dihydronepterin 2' :3'-cyclicphosphate + H2O -&gt; Dihydroneopterin phosphate + H+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dihydroneopterin phosphate + H2O &lt;=&gt; Dihydroneopterin + H+ + Ppi</t>
+  </si>
+  <si>
+    <t>Dihydroneopterin  -&gt; 6-hydroxymethyl-7,8-dihydropterin  + Glycolaldehyde</t>
+  </si>
+  <si>
+    <t>4-aminobenzoate + PRPP -&gt; beta-RFA-P</t>
+  </si>
+  <si>
+    <t>6-hydroxymethyl-7,8-dihydropterin + ATP -&gt; 6-hydroxymethyl-7,8-dihydropterin diphosphate + Ppi</t>
   </si>
 </sst>
 </file>
@@ -633,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,13 +1158,149 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="81.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Mfn but broken right now
</commit_message>
<xml_diff>
--- a/Matt_Work/Coenzyme Syntheses/synthesis pathway info.xlsx
+++ b/Matt_Work/Coenzyme Syntheses/synthesis pathway info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coenzyme B" sheetId="1" r:id="rId1"/>
@@ -712,12 +712,12 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1161,16 +1161,16 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="81.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1310,7 +1310,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>